<commit_message>
Added raw working photos
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E27C5E-08F0-4533-A8E2-26F3C50C5C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F928822F-DD26-4CC4-9350-1081C085BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Post Number</t>
   </si>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>In Queue</t>
+  </si>
+  <si>
+    <t>Scrubbed</t>
+  </si>
+  <si>
+    <t>Beach Rock</t>
+  </si>
+  <si>
+    <t>To many to count</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Sail Boats</t>
+  </si>
+  <si>
+    <t>Sunset</t>
+  </si>
+  <si>
+    <t>Water bowl</t>
+  </si>
+  <si>
+    <t>Tiny Waterfall</t>
   </si>
 </sst>
 </file>
@@ -446,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D3C61-D7FB-4931-8ABE-F8757006C31C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,8 +589,11 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -576,14 +603,72 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{50A0820B-AD85-46EA-B782-778C3F32E2E6}">
-      <formula1>"In Queue, Edited, Written, Posted"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30" xr:uid="{74793F9F-19DD-4DC1-A54E-7D3E958683D8}">
+      <formula1>"In Queue, Edited, Written, Posted, Scrubbed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some admin docs and sailboats post
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F928822F-DD26-4CC4-9350-1081C085BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734546DB-405B-4EE9-8C74-27F1E2703D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Post Number</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Posted</t>
   </si>
   <si>
-    <t>In Queue</t>
-  </si>
-  <si>
     <t>Scrubbed</t>
   </si>
   <si>
@@ -119,6 +116,12 @@
   </si>
   <si>
     <t>Tiny Waterfall</t>
+  </si>
+  <si>
+    <t>Edited</t>
+  </si>
+  <si>
+    <t>BeachRock.jpg</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,7 +593,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -604,10 +607,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -615,10 +618,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -626,10 +632,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -637,10 +643,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -648,10 +654,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -659,10 +665,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made some admin adjustments
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734546DB-405B-4EE9-8C74-27F1E2703D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24685F4-BA68-4405-ABCE-2D91BFC22925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
+    <workbookView xWindow="-8715" yWindow="3405" windowWidth="25590" windowHeight="15330" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Post Number</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>BeachRock.jpg</t>
+  </si>
+  <si>
+    <t>The Bahea</t>
+  </si>
+  <si>
+    <t>TheBahea.jpg</t>
   </si>
 </sst>
 </file>
@@ -473,21 +479,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D3C61-D7FB-4931-8ABE-F8757006C31C}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -515,7 +521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,7 +535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -543,7 +549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -557,7 +563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -571,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -585,7 +591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -599,7 +605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -613,7 +619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -627,7 +633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -635,10 +641,10 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -646,10 +652,10 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -657,10 +663,10 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -668,6 +674,20 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a BUNCH of photos
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3C0BDD-2C83-4F78-8F1E-5161F9188F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8044F5-FCDF-4A22-8397-E420F1C7DF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
+    <workbookView xWindow="10886" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Post Number</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Tiny Waterfall</t>
   </si>
   <si>
-    <t>Edited</t>
-  </si>
-  <si>
     <t>BeachRock.jpg</t>
   </si>
   <si>
@@ -128,6 +125,21 @@
   </si>
   <si>
     <t>On IG</t>
+  </si>
+  <si>
+    <t>Plane In the Clouds</t>
+  </si>
+  <si>
+    <t>Shot</t>
+  </si>
+  <si>
+    <t>Ausie Goose</t>
+  </si>
+  <si>
+    <t>Turtle on A Log</t>
+  </si>
+  <si>
+    <t>Squrille</t>
   </si>
 </sst>
 </file>
@@ -479,21 +491,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D3C61-D7FB-4931-8ABE-F8757006C31C}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,10 +530,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -532,10 +544,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -546,10 +558,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -560,10 +572,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -574,10 +586,10 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -588,10 +600,10 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -602,10 +614,10 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -619,7 +631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -627,13 +639,13 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -641,10 +653,10 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -652,10 +664,10 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -663,10 +675,10 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -674,21 +686,76 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed profile picture name
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C3564-4C35-4754-974C-F6F2B6549E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F94F023-6CD0-4189-B9BC-EC96BA389134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -686,7 +686,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
@@ -755,7 +755,7 @@
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scheduled a couple more posts
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F94F023-6CD0-4189-B9BC-EC96BA389134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45628966-A6A8-49A8-87AB-001D6133C2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Post Number</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>Duck on A Log</t>
+  </si>
+  <si>
+    <t>Ground Squirrel</t>
+  </si>
+  <si>
+    <t>Shot</t>
+  </si>
+  <si>
+    <t>Lady Quail</t>
   </si>
 </sst>
 </file>
@@ -491,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D3C61-D7FB-4931-8ABE-F8757006C31C}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -758,6 +767,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100" xr:uid="{CFE732E9-763F-4D43-93B8-A1EFEB0BDB7A}">

</xml_diff>

<commit_message>
Added some posts, pictures, and notes
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45628966-A6A8-49A8-87AB-001D6133C2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62FC2A-0A91-45C6-AC51-9688D64718E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Post Number</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Ground Squirrel</t>
-  </si>
-  <si>
-    <t>Shot</t>
   </si>
   <si>
     <t>Lady Quail</t>
@@ -503,7 +500,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -775,7 +772,7 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
@@ -783,16 +780,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100" xr:uid="{CFE732E9-763F-4D43-93B8-A1EFEB0BDB7A}">
-      <formula1>"In Queue, Designed, Shot, Edited, Written, Posted, On IG, Scrubbed"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D101" xr:uid="{E115D5EE-EE2C-4357-BA48-DFFD0D03F390}">
+      <formula1>"In Queue, Designed, Shot, Edited, Researched, Written, Posted, On IG, Scrubbed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added edited boat photo, updated schedule
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB44D5F-CF4B-4C3C-9511-9AD55FD44532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9D54A5-7F9F-4078-810F-BA5E50850F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +241,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -347,7 +347,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,7 +489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,18 +500,18 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -539,7 +539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -553,7 +553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -567,7 +567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -581,7 +581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -595,7 +595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -609,7 +609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -623,7 +623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -637,7 +637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -651,7 +651,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -662,7 +662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -673,7 +673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -684,7 +684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -695,7 +695,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -709,7 +709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -720,7 +720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -731,7 +731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -742,7 +742,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -753,7 +753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -764,7 +764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -775,7 +775,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Updated post schedule to account for finishing quail post
</commit_message>
<xml_diff>
--- a/PhotoBlogAdmin/PostSchedule.xlsx
+++ b/PhotoBlogAdmin/PostSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\PhotographyBlog\benbockphotography.github.io\PhotoBlogAdmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9D54A5-7F9F-4078-810F-BA5E50850F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB0E95-5A3F-4AFC-AC7E-92082CA333A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{178461E9-A359-476D-8F65-C13E7A039928}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +783,7 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>